<commit_message>
Admin Edit Movie Feature Added
</commit_message>
<xml_diff>
--- a/resources/BookMyShow.xlsx
+++ b/resources/BookMyShow.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbhurtel\PycharmProjects\PythonTrack_HU\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521D6BF7-E2BC-44CD-9C1C-98088FE2E1F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBBF1431-7CFD-4215-894C-F481E87A8E01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="990" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{129A9AA1-7AC5-46DF-83D3-F055B7B02343}"/>
+    <workbookView xWindow="340" yWindow="2290" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{129A9AA1-7AC5-46DF-83D3-F055B7B02343}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCredentials" sheetId="3" r:id="rId1"/>
     <sheet name="UserDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="Movies" sheetId="6" r:id="rId3"/>
+    <sheet name="Movie_list" sheetId="7" r:id="rId3"/>
     <sheet name="Ratings" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
@@ -109,6 +109,39 @@
   </si>
   <si>
     <t>Tes</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>2hr 30m</t>
+  </si>
+  <si>
+    <t>Robert Jr.</t>
+  </si>
+  <si>
+    <t>Stan lee</t>
+  </si>
+  <si>
+    <t>Eng</t>
+  </si>
+  <si>
+    <t>8h 0m</t>
+  </si>
+  <si>
+    <t>0h 30m</t>
+  </si>
+  <si>
+    <t>0h 15min</t>
+  </si>
+  <si>
+    <t>1-2 2-3</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
@@ -502,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869839AA-D17B-4083-B1F5-5C8BFB9C303D}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,11 +567,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256FD329-F5AC-48C6-A477-B07176173E0A}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7533FBE8-7CFD-4325-A061-660BCA8F97E3}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,6 +615,88 @@
       </c>
       <c r="M1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>3.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>3.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>